<commit_message>
revised NCNO tab to be clearer, provided context
</commit_message>
<xml_diff>
--- a/NCNO.xlsx
+++ b/NCNO.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/specter/USEquities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A1EAF5-5B2F-C743-B258-1E0AA22DE50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0A6336-70DB-7A44-AEBC-22EA179D7A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Landing Page" sheetId="4" r:id="rId1"/>
     <sheet name="P_S ratio Estimates (8.9.22)" sheetId="2" r:id="rId2"/>
-    <sheet name="P_S ratio Estimates (9.1.22)" sheetId="3" r:id="rId3"/>
+    <sheet name="P_S ratio Estimates (8.9.22(2))" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="171">
   <si>
     <t>Valuation Options: :</t>
   </si>
@@ -543,19 +543,28 @@
     <t>Quarterly change in TTM rev (est)</t>
   </si>
   <si>
-    <t>Narrative: 
-The Teal range shown in the P/S ratio tabs show the range for the trading period POST earnings indicated.</t>
+    <t>Revenues:</t>
+  </si>
+  <si>
+    <t>Narrative: NCNO has lumpy quarterly growth, but the growth in TTM revenue is steady. The estimations accomadate this by driving calculations off of TTM. 
+How To Use:
+The name of the tab represents the last date the tab was updated, viewers should use the latest estimate tab. 
+The top section represents Revenues, the second section is a matrix plotting a price to sales ratio against the actual trading price and estimated or actual revenues. 
+Revenue Section - The revenue section uses actual data as available and estimates using growth where not possible. TTM deltas for each non guidance quarter is estimated by averaging the previous 8 quarterly TTM change in revenue. This drives the value for estimated TTM, as well as quarterly revenue and growth estimates.
+The Orange highlights represent Guidance Values
+The Teal range shown in the P/S ratio shows the price range for the trading period after the earnings announcement.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mmm\ d\ yyyy"/>
     <numFmt numFmtId="165" formatCode="mmmm\ d\ yyyy"/>
+    <numFmt numFmtId="168" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -594,8 +603,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,6 +652,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -743,10 +771,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -918,12 +947,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1138,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBD4608-881B-F34A-AB93-66622F7714D7}">
   <dimension ref="A1:X1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1150,8 +1206,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="61" t="s">
-        <v>169</v>
+      <c r="A1" s="63" t="s">
+        <v>170</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -11651,13 +11707,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA93297A-2586-FC44-93EE-DC8E2BBA76BC}">
   <dimension ref="A2:V32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22">
@@ -13895,2246 +13962,1832 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D192A948-EC69-C348-809B-D483196A31C3}">
-  <dimension ref="A2:V32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95121430-7F97-D540-A51A-DC143E1D3CA7}">
+  <dimension ref="A3:V28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="59" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="59"/>
+    <col min="2" max="2" width="11" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11" style="59" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="59" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11" style="59" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="59" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="11" style="59" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" style="59" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="11" style="59" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" style="59" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="11" style="59" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="10.83203125" style="59"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22">
-      <c r="A2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="3"/>
-      <c r="G2" s="3" t="s">
+    <row r="3" spans="1:22">
+      <c r="A3" s="61" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="3"/>
+      <c r="G3" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12" t="s">
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="14" t="s">
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P4" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q4" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="R4" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="S4" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="T4" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="U3" s="17" t="s">
+      <c r="U4" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="V4" s="17" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="P4" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="R4" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="S4" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="T4" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="V4" s="12" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="21">
-        <v>43496</v>
-      </c>
-      <c r="C5" s="22">
-        <v>43585</v>
-      </c>
-      <c r="D5" s="21">
-        <v>43677</v>
-      </c>
-      <c r="E5" s="21">
-        <v>43769</v>
-      </c>
-      <c r="F5" s="21">
-        <v>43861</v>
-      </c>
-      <c r="G5" s="22">
-        <v>43951</v>
-      </c>
-      <c r="H5" s="21">
-        <v>44043</v>
-      </c>
-      <c r="I5" s="21">
-        <v>44135</v>
-      </c>
-      <c r="J5" s="21">
-        <v>44227</v>
-      </c>
-      <c r="K5" s="22">
-        <v>44316</v>
-      </c>
-      <c r="L5" s="21">
-        <v>44408</v>
-      </c>
-      <c r="M5" s="21">
-        <v>44500</v>
-      </c>
-      <c r="N5" s="21">
-        <v>44592</v>
-      </c>
-      <c r="O5" s="45">
-        <v>44681</v>
-      </c>
-      <c r="P5" s="46">
-        <v>44773</v>
-      </c>
-      <c r="Q5" s="44">
-        <v>44865</v>
-      </c>
-      <c r="R5" s="44">
-        <v>44957</v>
-      </c>
-      <c r="S5" s="45">
-        <v>45046</v>
-      </c>
-      <c r="T5" s="44">
-        <v>45138</v>
-      </c>
-      <c r="U5" s="44">
-        <v>45230</v>
-      </c>
-      <c r="V5" s="44">
-        <v>45322</v>
+        <v>111</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="P5" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="U5" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="V5" s="12" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="13">
-        <v>29836</v>
-      </c>
-      <c r="D6" s="13">
-        <v>31978</v>
-      </c>
-      <c r="E6" s="13">
-        <v>37862</v>
-      </c>
-      <c r="F6" s="30">
-        <v>38504</v>
-      </c>
-      <c r="G6" s="13">
-        <v>44712</v>
-      </c>
-      <c r="H6" s="27">
-        <v>48765</v>
-      </c>
-      <c r="I6" s="13">
-        <v>54229</v>
-      </c>
-      <c r="J6" s="13">
-        <v>56587</v>
-      </c>
-      <c r="K6" s="13">
-        <v>62355</v>
-      </c>
-      <c r="L6" s="13">
-        <v>66519</v>
-      </c>
-      <c r="M6" s="13">
-        <v>70036</v>
-      </c>
-      <c r="N6" s="3">
-        <v>74955</v>
-      </c>
-      <c r="O6" s="12">
-        <v>94200</v>
-      </c>
-      <c r="P6" s="28">
-        <v>97500</v>
-      </c>
-      <c r="Q6" s="29">
-        <f t="shared" ref="Q6:V6" si="0">Q29</f>
-        <v>100338.19</v>
-      </c>
-      <c r="R6" s="29">
-        <f t="shared" si="0"/>
-        <v>109961.81</v>
-      </c>
-      <c r="S6" s="29">
-        <f t="shared" si="0"/>
-        <v>130380.00000000006</v>
-      </c>
-      <c r="T6" s="29">
-        <f t="shared" si="0"/>
-        <v>136936.20000000001</v>
-      </c>
-      <c r="U6" s="29">
-        <f t="shared" si="0"/>
-        <v>143323.64800000004</v>
-      </c>
-      <c r="V6" s="29">
-        <f t="shared" si="0"/>
-        <v>156815.95922000008</v>
+        <v>133</v>
+      </c>
+      <c r="B6" s="21">
+        <v>43496</v>
+      </c>
+      <c r="C6" s="22">
+        <v>43585</v>
+      </c>
+      <c r="D6" s="21">
+        <v>43677</v>
+      </c>
+      <c r="E6" s="21">
+        <v>43769</v>
+      </c>
+      <c r="F6" s="21">
+        <v>43861</v>
+      </c>
+      <c r="G6" s="22">
+        <v>43951</v>
+      </c>
+      <c r="H6" s="21">
+        <v>44043</v>
+      </c>
+      <c r="I6" s="21">
+        <v>44135</v>
+      </c>
+      <c r="J6" s="21">
+        <v>44227</v>
+      </c>
+      <c r="K6" s="22">
+        <v>44316</v>
+      </c>
+      <c r="L6" s="21">
+        <v>44408</v>
+      </c>
+      <c r="M6" s="21">
+        <v>44500</v>
+      </c>
+      <c r="N6" s="21">
+        <v>44592</v>
+      </c>
+      <c r="O6" s="45">
+        <v>44681</v>
+      </c>
+      <c r="P6" s="46">
+        <v>44773</v>
+      </c>
+      <c r="Q6" s="44">
+        <v>44865</v>
+      </c>
+      <c r="R6" s="44">
+        <v>44957</v>
+      </c>
+      <c r="S6" s="45">
+        <v>45046</v>
+      </c>
+      <c r="T6" s="44">
+        <v>45138</v>
+      </c>
+      <c r="U6" s="44">
+        <v>45230</v>
+      </c>
+      <c r="V6" s="44">
+        <v>45322</v>
       </c>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="13">
+        <v>29836</v>
+      </c>
+      <c r="D7" s="13">
+        <v>31978</v>
+      </c>
+      <c r="E7" s="13">
+        <v>37862</v>
+      </c>
+      <c r="F7" s="30">
+        <v>38504</v>
+      </c>
+      <c r="G7" s="13">
+        <v>44712</v>
+      </c>
+      <c r="H7" s="27">
+        <v>48765</v>
+      </c>
+      <c r="I7" s="13">
+        <v>54229</v>
+      </c>
+      <c r="J7" s="13">
+        <v>56587</v>
+      </c>
+      <c r="K7" s="13">
+        <v>62355</v>
+      </c>
+      <c r="L7" s="13">
+        <v>66519</v>
+      </c>
+      <c r="M7" s="13">
+        <v>70036</v>
+      </c>
+      <c r="N7" s="3">
+        <v>74955</v>
+      </c>
+      <c r="O7" s="12">
+        <v>94200</v>
+      </c>
+      <c r="P7" s="28">
+        <v>97500</v>
+      </c>
+      <c r="Q7" s="70">
+        <f>Q8-SUM(N7:P7)</f>
+        <v>100140.11229027284</v>
+      </c>
+      <c r="R7" s="70">
+        <f t="shared" ref="R7:V7" si="0">R8-SUM(O7:Q7)</f>
+        <v>110159.88770972716</v>
+      </c>
+      <c r="S7" s="70">
+        <f t="shared" si="0"/>
+        <v>129363.51542796066</v>
+      </c>
+      <c r="T7" s="70">
+        <f t="shared" si="0"/>
+        <v>135799.98449849006</v>
+      </c>
+      <c r="U7" s="70">
+        <f t="shared" si="0"/>
+        <v>142248.09862020449</v>
+      </c>
+      <c r="V7" s="70">
+        <f t="shared" si="0"/>
+        <v>157460.10454047093</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="30">
-        <f t="shared" ref="F7:P7" si="1">C6+D6+E6+F6</f>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="30">
+        <f t="shared" ref="F8:P8" si="1">C7+D7+E7+F7</f>
         <v>138180</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G8" s="30">
         <f t="shared" si="1"/>
         <v>153056</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H8" s="30">
         <f t="shared" si="1"/>
         <v>169843</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I8" s="30">
         <f t="shared" si="1"/>
         <v>186210</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J8" s="30">
         <f t="shared" si="1"/>
         <v>204293</v>
       </c>
-      <c r="K7" s="30">
+      <c r="K8" s="30">
         <f t="shared" si="1"/>
         <v>221936</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L8" s="30">
         <f t="shared" si="1"/>
         <v>239690</v>
       </c>
-      <c r="M7" s="30">
+      <c r="M8" s="30">
         <f t="shared" si="1"/>
         <v>255497</v>
       </c>
-      <c r="N7" s="30">
+      <c r="N8" s="30">
         <f t="shared" si="1"/>
         <v>273865</v>
       </c>
-      <c r="O7" s="31">
+      <c r="O8" s="31">
         <f t="shared" si="1"/>
         <v>305710</v>
       </c>
-      <c r="P7" s="32">
+      <c r="P8" s="32">
         <f t="shared" si="1"/>
         <v>336691</v>
       </c>
-      <c r="Q7" s="33">
-        <f t="shared" ref="Q7:V7" si="2">Q31</f>
-        <v>366993.19</v>
-      </c>
-      <c r="R7" s="52">
+      <c r="Q8" s="69">
+        <f>P8*(1+Q10)</f>
+        <v>366795.11229027284</v>
+      </c>
+      <c r="R8" s="69">
+        <v>402000</v>
+      </c>
+      <c r="S8" s="69">
+        <f t="shared" ref="R8:V8" si="2">R8*(1+S10)</f>
+        <v>437163.51542796066</v>
+      </c>
+      <c r="T8" s="69">
         <f t="shared" si="2"/>
-        <v>402000</v>
-      </c>
-      <c r="S7" s="33">
+        <v>475463.49992645072</v>
+      </c>
+      <c r="U8" s="69">
         <f t="shared" si="2"/>
-        <v>438180.00000000006</v>
-      </c>
-      <c r="T7" s="33">
+        <v>517571.48625638237</v>
+      </c>
+      <c r="V8" s="69">
         <f t="shared" si="2"/>
-        <v>477616.20000000007</v>
-      </c>
-      <c r="U7" s="33">
-        <f t="shared" si="2"/>
-        <v>520601.65800000011</v>
-      </c>
-      <c r="V7" s="33">
-        <f t="shared" si="2"/>
-        <v>567455.80722000019</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="P8" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3">
-        <f t="shared" ref="D10:V10" si="3">D7*5/96750</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
+        <v>564871.70308712614</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="65" customFormat="1">
+      <c r="A9" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64">
+        <f>(D7-C7)/C7</f>
+        <v>7.1792465477946099E-2</v>
+      </c>
+      <c r="E9" s="64">
+        <f t="shared" ref="E9:V9" si="3">(E7-D7)/D7</f>
+        <v>0.18400150103195947</v>
+      </c>
+      <c r="F9" s="64">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
+        <v>1.6956315038825207E-2</v>
+      </c>
+      <c r="G9" s="64">
         <f t="shared" si="3"/>
-        <v>7.1410852713178299</v>
-      </c>
-      <c r="G10" s="3">
+        <v>0.16123000207770621</v>
+      </c>
+      <c r="H9" s="64">
         <f t="shared" si="3"/>
-        <v>7.9098708010335921</v>
-      </c>
-      <c r="H10" s="3">
+        <v>9.0646806226516372E-2</v>
+      </c>
+      <c r="I9" s="64">
         <f t="shared" si="3"/>
-        <v>8.7774160206718346</v>
-      </c>
-      <c r="I10" s="3">
+        <v>0.11204757510509587</v>
+      </c>
+      <c r="J9" s="64">
         <f t="shared" si="3"/>
-        <v>9.6232558139534881</v>
-      </c>
-      <c r="J10" s="3">
+        <v>4.3482269634328496E-2</v>
+      </c>
+      <c r="K9" s="64">
         <f t="shared" si="3"/>
-        <v>10.557777777777778</v>
-      </c>
-      <c r="K10" s="3">
+        <v>0.10193153904607065</v>
+      </c>
+      <c r="L9" s="64">
         <f t="shared" si="3"/>
-        <v>11.469560723514212</v>
-      </c>
-      <c r="L10" s="3">
+        <v>6.6778927110897279E-2</v>
+      </c>
+      <c r="M9" s="64">
         <f t="shared" si="3"/>
-        <v>12.387080103359173</v>
-      </c>
-      <c r="M10" s="3">
+        <v>5.2872111727476363E-2</v>
+      </c>
+      <c r="N9" s="64">
         <f t="shared" si="3"/>
-        <v>13.203979328165374</v>
-      </c>
-      <c r="N10" s="3">
+        <v>7.0235307556113999E-2</v>
+      </c>
+      <c r="O9" s="64">
         <f t="shared" si="3"/>
-        <v>14.153229974160206</v>
-      </c>
-      <c r="O10" s="12">
+        <v>0.25675405243145888</v>
+      </c>
+      <c r="P9" s="64">
         <f t="shared" si="3"/>
-        <v>15.798966408268734</v>
-      </c>
-      <c r="P10" s="35">
+        <v>3.5031847133757961E-2</v>
+      </c>
+      <c r="Q9" s="64">
         <f t="shared" si="3"/>
-        <v>17.400051679586564</v>
-      </c>
-      <c r="Q10" s="12">
+        <v>2.7078074772029111E-2</v>
+      </c>
+      <c r="R9" s="64">
         <f t="shared" si="3"/>
-        <v>18.966056330749353</v>
-      </c>
-      <c r="R10" s="12">
+        <v>0.10005756125387927</v>
+      </c>
+      <c r="S9" s="64">
         <f t="shared" si="3"/>
-        <v>20.775193798449614</v>
-      </c>
-      <c r="S10" s="12">
+        <v>0.17432504805047849</v>
+      </c>
+      <c r="T9" s="64">
         <f t="shared" si="3"/>
-        <v>22.644961240310082</v>
-      </c>
-      <c r="T10" s="12">
+        <v>4.9754902294021998E-2</v>
+      </c>
+      <c r="U9" s="64">
         <f t="shared" si="3"/>
-        <v>24.683007751937989</v>
-      </c>
-      <c r="U10" s="12">
+        <v>4.748243636055885E-2</v>
+      </c>
+      <c r="V9" s="64">
         <f t="shared" si="3"/>
-        <v>26.904478449612409</v>
-      </c>
-      <c r="V10" s="12">
-        <f t="shared" si="3"/>
-        <v>29.325881510077529</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3">
-        <f t="shared" ref="F11:V11" si="4">F7*7.5/96750</f>
-        <v>10.711627906976744</v>
-      </c>
-      <c r="G11" s="3">
+        <v>0.10693995960453404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" s="65" customFormat="1">
+      <c r="A10" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64">
+        <f>(G8-F8)/F8</f>
+        <v>0.10765667969315386</v>
+      </c>
+      <c r="H10" s="64">
+        <f t="shared" ref="H10:P10" si="4">(H8-G8)/G8</f>
+        <v>0.10967881037006064</v>
+      </c>
+      <c r="I10" s="64">
         <f t="shared" si="4"/>
-        <v>11.864806201550387</v>
-      </c>
-      <c r="H11" s="3">
+        <v>9.6365466931224719E-2</v>
+      </c>
+      <c r="J10" s="64">
         <f t="shared" si="4"/>
-        <v>13.166124031007753</v>
-      </c>
-      <c r="I11" s="3">
+        <v>9.711078889425917E-2</v>
+      </c>
+      <c r="K10" s="64">
         <f t="shared" si="4"/>
-        <v>14.434883720930232</v>
-      </c>
-      <c r="J11" s="3">
+        <v>8.6361255647525864E-2</v>
+      </c>
+      <c r="L10" s="64">
         <f t="shared" si="4"/>
-        <v>15.836666666666666</v>
-      </c>
-      <c r="K11" s="3">
+        <v>7.9996034892942103E-2</v>
+      </c>
+      <c r="M10" s="64">
         <f t="shared" si="4"/>
-        <v>17.204341085271317</v>
-      </c>
-      <c r="L11" s="3">
+        <v>6.5947682423129872E-2</v>
+      </c>
+      <c r="N10" s="64">
         <f t="shared" si="4"/>
-        <v>18.580620155038758</v>
-      </c>
-      <c r="M11" s="3">
+        <v>7.1891255083229938E-2</v>
+      </c>
+      <c r="O10" s="64">
         <f t="shared" si="4"/>
-        <v>19.805968992248062</v>
-      </c>
-      <c r="N11" s="38">
+        <v>0.11627991893816296</v>
+      </c>
+      <c r="P10" s="64">
         <f t="shared" si="4"/>
-        <v>21.22984496124031</v>
-      </c>
-      <c r="O11" s="38">
-        <f t="shared" si="4"/>
-        <v>23.698449612403103</v>
-      </c>
-      <c r="P11" s="37">
-        <f t="shared" si="4"/>
-        <v>26.100077519379845</v>
-      </c>
-      <c r="Q11" s="3">
-        <f t="shared" si="4"/>
-        <v>28.44908449612403</v>
-      </c>
-      <c r="R11" s="3">
-        <f t="shared" si="4"/>
-        <v>31.162790697674417</v>
-      </c>
-      <c r="S11" s="3">
-        <f t="shared" si="4"/>
-        <v>33.967441860465122</v>
-      </c>
-      <c r="T11" s="3">
-        <f t="shared" si="4"/>
-        <v>37.024511627906982</v>
-      </c>
-      <c r="U11" s="3">
-        <f t="shared" si="4"/>
-        <v>40.356717674418611</v>
-      </c>
-      <c r="V11" s="3">
-        <f t="shared" si="4"/>
-        <v>43.988822265116291</v>
-      </c>
+        <v>0.10134114029635929</v>
+      </c>
+      <c r="Q10" s="71">
+        <f>(AVERAGE(I10:P10))</f>
+        <v>8.9411692888354238E-2</v>
+      </c>
+      <c r="R10" s="71">
+        <f t="shared" ref="R10:V10" si="5">(AVERAGE(J10:Q10))</f>
+        <v>8.8542471132995432E-2</v>
+      </c>
+      <c r="S10" s="71">
+        <f t="shared" si="5"/>
+        <v>8.7471431412837461E-2</v>
+      </c>
+      <c r="T10" s="71">
+        <f t="shared" si="5"/>
+        <v>8.7610203383501409E-2</v>
+      </c>
+      <c r="U10" s="71">
+        <f t="shared" si="5"/>
+        <v>8.856197444482132E-2</v>
+      </c>
+      <c r="V10" s="71">
+        <f t="shared" si="5"/>
+        <v>9.1388760947532746E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="65" customFormat="1">
+      <c r="A11" s="62"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="67"/>
+      <c r="R11" s="67"/>
+      <c r="S11" s="67"/>
+      <c r="T11" s="67"/>
+      <c r="U11" s="67"/>
+      <c r="V11" s="67"/>
     </row>
     <row r="12" spans="1:22">
-      <c r="A12" s="18" t="s">
-        <v>153</v>
+      <c r="A12" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3">
-        <f t="shared" ref="D12:V12" si="5">D7*10/96750</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" si="5"/>
-        <v>14.28217054263566</v>
-      </c>
-      <c r="G12" s="3">
-        <f t="shared" si="5"/>
-        <v>15.819741602067184</v>
-      </c>
-      <c r="H12" s="3">
-        <f t="shared" si="5"/>
-        <v>17.554832041343669</v>
-      </c>
-      <c r="I12" s="3">
-        <f t="shared" si="5"/>
-        <v>19.246511627906976</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="5"/>
-        <v>21.115555555555556</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" si="5"/>
-        <v>22.939121447028423</v>
-      </c>
-      <c r="L12" s="3">
-        <f t="shared" si="5"/>
-        <v>24.774160206718346</v>
-      </c>
-      <c r="M12" s="12">
-        <f t="shared" si="5"/>
-        <v>26.407958656330749</v>
-      </c>
-      <c r="N12" s="38">
-        <f t="shared" si="5"/>
-        <v>28.306459948320413</v>
-      </c>
-      <c r="O12" s="38">
-        <f t="shared" si="5"/>
-        <v>31.597932816537469</v>
-      </c>
-      <c r="P12" s="35">
-        <f t="shared" si="5"/>
-        <v>34.800103359173129</v>
-      </c>
-      <c r="Q12" s="12">
-        <f t="shared" si="5"/>
-        <v>37.932112661498707</v>
-      </c>
-      <c r="R12" s="12">
-        <f t="shared" si="5"/>
-        <v>41.550387596899228</v>
-      </c>
-      <c r="S12" s="12">
-        <f t="shared" si="5"/>
-        <v>45.289922480620163</v>
-      </c>
-      <c r="T12" s="12">
-        <f t="shared" si="5"/>
-        <v>49.366015503875978</v>
-      </c>
-      <c r="U12" s="12">
-        <f t="shared" si="5"/>
-        <v>53.808956899224818</v>
-      </c>
-      <c r="V12" s="12">
-        <f t="shared" si="5"/>
-        <v>58.651763020155059</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
-      <c r="A13" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3">
-        <f t="shared" ref="F13:V13" si="6">F7*12.5/96750</f>
-        <v>17.852713178294575</v>
-      </c>
-      <c r="G13" s="3">
-        <f t="shared" si="6"/>
-        <v>19.774677002583978</v>
-      </c>
-      <c r="H13" s="3">
-        <f t="shared" si="6"/>
-        <v>21.943540051679587</v>
-      </c>
-      <c r="I13" s="3">
-        <f t="shared" si="6"/>
-        <v>24.058139534883722</v>
-      </c>
-      <c r="J13" s="3">
-        <f t="shared" si="6"/>
-        <v>26.394444444444446</v>
-      </c>
-      <c r="K13" s="3">
-        <f t="shared" si="6"/>
-        <v>28.67390180878553</v>
-      </c>
-      <c r="L13" s="3">
-        <f t="shared" si="6"/>
-        <v>30.967700258397933</v>
-      </c>
-      <c r="M13" s="38">
-        <f t="shared" si="6"/>
-        <v>33.009948320413436</v>
-      </c>
-      <c r="N13" s="38">
-        <f t="shared" si="6"/>
-        <v>35.383074935400515</v>
-      </c>
-      <c r="O13" s="38">
-        <f t="shared" si="6"/>
-        <v>39.497416020671835</v>
-      </c>
-      <c r="P13" s="37">
-        <f t="shared" si="6"/>
-        <v>43.500129198966405</v>
-      </c>
-      <c r="Q13" s="3">
-        <f t="shared" si="6"/>
-        <v>47.415140826873383</v>
-      </c>
-      <c r="R13" s="3">
-        <f t="shared" si="6"/>
-        <v>51.937984496124031</v>
-      </c>
-      <c r="S13" s="3">
-        <f t="shared" si="6"/>
-        <v>56.612403100775204</v>
-      </c>
-      <c r="T13" s="3">
-        <f t="shared" si="6"/>
-        <v>61.707519379844967</v>
-      </c>
-      <c r="U13" s="3">
-        <f t="shared" si="6"/>
-        <v>67.261196124031017</v>
-      </c>
-      <c r="V13" s="3">
-        <f t="shared" si="6"/>
-        <v>73.31470377519382</v>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="68"/>
+      <c r="Q12" s="69"/>
+      <c r="R12" s="69"/>
+      <c r="S12" s="69"/>
+      <c r="T12" s="69"/>
+      <c r="U12" s="69"/>
+      <c r="V12" s="69"/>
+    </row>
+    <row r="13" spans="1:22" s="61" customFormat="1">
+      <c r="A13" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="P13" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:22">
-      <c r="A14" s="18" t="s">
-        <v>155</v>
+      <c r="A14" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3">
-        <f t="shared" ref="D14:V14" si="7">D7*15/96750</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" si="7"/>
-        <v>21.423255813953489</v>
-      </c>
-      <c r="G14" s="3">
-        <f t="shared" si="7"/>
-        <v>23.729612403100774</v>
-      </c>
-      <c r="H14" s="3">
-        <f t="shared" si="7"/>
-        <v>26.332248062015505</v>
-      </c>
-      <c r="I14" s="3">
-        <f t="shared" si="7"/>
-        <v>28.869767441860464</v>
-      </c>
-      <c r="J14" s="3">
-        <f t="shared" si="7"/>
-        <v>31.673333333333332</v>
-      </c>
-      <c r="K14" s="3">
-        <f t="shared" si="7"/>
-        <v>34.408682170542633</v>
-      </c>
-      <c r="L14" s="3">
-        <f t="shared" si="7"/>
-        <v>37.161240310077517</v>
-      </c>
-      <c r="M14" s="38">
-        <f t="shared" si="7"/>
-        <v>39.611937984496123</v>
-      </c>
-      <c r="N14" s="38">
-        <f t="shared" si="7"/>
-        <v>42.459689922480621</v>
-      </c>
-      <c r="O14" s="12">
-        <f t="shared" si="7"/>
-        <v>47.396899224806205</v>
-      </c>
-      <c r="P14" s="35">
-        <f t="shared" si="7"/>
-        <v>52.200155038759689</v>
-      </c>
-      <c r="Q14" s="12">
-        <f t="shared" si="7"/>
-        <v>56.89816899224806</v>
-      </c>
-      <c r="R14" s="12">
-        <f t="shared" si="7"/>
-        <v>62.325581395348834</v>
-      </c>
-      <c r="S14" s="12">
-        <f t="shared" si="7"/>
-        <v>67.934883720930245</v>
-      </c>
-      <c r="T14" s="12">
-        <f t="shared" si="7"/>
-        <v>74.049023255813964</v>
-      </c>
-      <c r="U14" s="12">
-        <f t="shared" si="7"/>
-        <v>80.713435348837223</v>
-      </c>
-      <c r="V14" s="12">
-        <f t="shared" si="7"/>
-        <v>87.977644530232581</v>
-      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="18" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="3">
+        <f>D8*5/96750</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <f>E8*5/96750</f>
+        <v>0</v>
+      </c>
       <c r="F15" s="3">
-        <f t="shared" ref="F15:V15" si="8">F7*17.5/96750</f>
-        <v>24.993798449612402</v>
+        <f>F8*5/96750</f>
+        <v>7.1410852713178299</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="8"/>
-        <v>27.684547803617573</v>
+        <f>G8*5/96750</f>
+        <v>7.9098708010335921</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="8"/>
-        <v>30.72095607235142</v>
+        <f>H8*5/96750</f>
+        <v>8.7774160206718346</v>
       </c>
       <c r="I15" s="3">
-        <f t="shared" si="8"/>
-        <v>33.681395348837206</v>
-      </c>
-      <c r="J15" s="38">
-        <f t="shared" si="8"/>
-        <v>36.952222222222225</v>
+        <f>I8*5/96750</f>
+        <v>9.6232558139534881</v>
+      </c>
+      <c r="J15" s="3">
+        <f>J8*5/96750</f>
+        <v>10.557777777777778</v>
       </c>
       <c r="K15" s="3">
-        <f t="shared" si="8"/>
-        <v>40.143462532299743</v>
+        <f>K8*5/96750</f>
+        <v>11.469560723514212</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" si="8"/>
-        <v>43.354780361757108</v>
-      </c>
-      <c r="M15" s="38">
-        <f t="shared" si="8"/>
-        <v>46.21392764857881</v>
+        <f>L8*5/96750</f>
+        <v>12.387080103359173</v>
+      </c>
+      <c r="M15" s="3">
+        <f>M8*5/96750</f>
+        <v>13.203979328165374</v>
       </c>
       <c r="N15" s="3">
-        <f t="shared" si="8"/>
-        <v>49.536304909560727</v>
-      </c>
-      <c r="O15" s="3">
-        <f t="shared" si="8"/>
-        <v>55.296382428940568</v>
-      </c>
-      <c r="P15" s="37">
-        <f t="shared" si="8"/>
-        <v>60.900180878552973</v>
-      </c>
-      <c r="Q15" s="3">
-        <f t="shared" si="8"/>
-        <v>66.381197157622736</v>
-      </c>
-      <c r="R15" s="3">
-        <f t="shared" si="8"/>
-        <v>72.713178294573638</v>
-      </c>
-      <c r="S15" s="3">
-        <f t="shared" si="8"/>
-        <v>79.257364341085278</v>
-      </c>
-      <c r="T15" s="3">
-        <f t="shared" si="8"/>
-        <v>86.39052713178296</v>
-      </c>
-      <c r="U15" s="3">
-        <f t="shared" si="8"/>
-        <v>94.165674573643443</v>
-      </c>
-      <c r="V15" s="3">
-        <f t="shared" si="8"/>
-        <v>102.64058528527136</v>
+        <f>N8*5/96750</f>
+        <v>14.153229974160206</v>
+      </c>
+      <c r="O15" s="12">
+        <f>O8*5/96750</f>
+        <v>15.798966408268734</v>
+      </c>
+      <c r="P15" s="35">
+        <f>P8*5/96750</f>
+        <v>17.400051679586564</v>
+      </c>
+      <c r="Q15" s="12">
+        <f>Q8*5/96750</f>
+        <v>18.955819756603248</v>
+      </c>
+      <c r="R15" s="12">
+        <f>R8*5/96750</f>
+        <v>20.775193798449614</v>
+      </c>
+      <c r="S15" s="12">
+        <f>S8*5/96750</f>
+        <v>22.592429737879105</v>
+      </c>
+      <c r="T15" s="12">
+        <f>T8*5/96750</f>
+        <v>24.571757102142158</v>
+      </c>
+      <c r="U15" s="12">
+        <f>U8*5/96750</f>
+        <v>26.747880426686425</v>
+      </c>
+      <c r="V15" s="12">
+        <f>V8*5/96750</f>
+        <v>29.192336076854062</v>
       </c>
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="18" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="3">
-        <f t="shared" ref="D16:V16" si="9">D7*20/96750</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="3">
-        <f t="shared" si="9"/>
-        <v>28.56434108527132</v>
+        <f>F8*7.5/96750</f>
+        <v>10.711627906976744</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="9"/>
-        <v>31.639483204134368</v>
+        <f>G8*7.5/96750</f>
+        <v>11.864806201550387</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="9"/>
-        <v>35.109664082687338</v>
+        <f>H8*7.5/96750</f>
+        <v>13.166124031007753</v>
       </c>
       <c r="I16" s="3">
-        <f t="shared" si="9"/>
-        <v>38.493023255813952</v>
-      </c>
-      <c r="J16" s="38">
-        <f t="shared" si="9"/>
-        <v>42.231111111111112</v>
+        <f>I8*7.5/96750</f>
+        <v>14.434883720930232</v>
+      </c>
+      <c r="J16" s="3">
+        <f>J8*7.5/96750</f>
+        <v>15.836666666666666</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" si="9"/>
-        <v>45.878242894056847</v>
-      </c>
-      <c r="L16" s="38">
-        <f t="shared" si="9"/>
-        <v>49.548320413436691</v>
-      </c>
-      <c r="M16" s="38">
-        <f t="shared" si="9"/>
-        <v>52.815917312661497</v>
-      </c>
-      <c r="N16" s="3">
-        <f t="shared" si="9"/>
-        <v>56.612919896640825</v>
-      </c>
-      <c r="O16" s="12">
-        <f t="shared" si="9"/>
-        <v>63.195865633074938</v>
-      </c>
-      <c r="P16" s="35">
-        <f t="shared" si="9"/>
-        <v>69.600206718346257</v>
-      </c>
-      <c r="Q16" s="12">
-        <f t="shared" si="9"/>
-        <v>75.864225322997413</v>
-      </c>
-      <c r="R16" s="12">
-        <f t="shared" si="9"/>
-        <v>83.100775193798455</v>
-      </c>
-      <c r="S16" s="12">
-        <f t="shared" si="9"/>
-        <v>90.579844961240326</v>
-      </c>
-      <c r="T16" s="12">
-        <f t="shared" si="9"/>
-        <v>98.732031007751957</v>
-      </c>
-      <c r="U16" s="12">
-        <f t="shared" si="9"/>
-        <v>107.61791379844964</v>
-      </c>
-      <c r="V16" s="12">
-        <f t="shared" si="9"/>
-        <v>117.30352604031012</v>
+        <f>K8*7.5/96750</f>
+        <v>17.204341085271317</v>
+      </c>
+      <c r="L16" s="3">
+        <f>L8*7.5/96750</f>
+        <v>18.580620155038758</v>
+      </c>
+      <c r="M16" s="3">
+        <f>M8*7.5/96750</f>
+        <v>19.805968992248062</v>
+      </c>
+      <c r="N16" s="38">
+        <f>N8*7.5/96750</f>
+        <v>21.22984496124031</v>
+      </c>
+      <c r="O16" s="38">
+        <f>O8*7.5/96750</f>
+        <v>23.698449612403103</v>
+      </c>
+      <c r="P16" s="37">
+        <f>P8*7.5/96750</f>
+        <v>26.100077519379845</v>
+      </c>
+      <c r="Q16" s="3">
+        <f>Q8*7.5/96750</f>
+        <v>28.433729634904871</v>
+      </c>
+      <c r="R16" s="3">
+        <f>R8*7.5/96750</f>
+        <v>31.162790697674417</v>
+      </c>
+      <c r="S16" s="3">
+        <f>S8*7.5/96750</f>
+        <v>33.888644606818652</v>
+      </c>
+      <c r="T16" s="3">
+        <f>T8*7.5/96750</f>
+        <v>36.857635653213237</v>
+      </c>
+      <c r="U16" s="3">
+        <f>U8*7.5/96750</f>
+        <v>40.12182064002964</v>
+      </c>
+      <c r="V16" s="3">
+        <f>V8*7.5/96750</f>
+        <v>43.788504115281093</v>
       </c>
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="18" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="D17" s="3">
+        <f>D8*10/96750</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <f>E8*10/96750</f>
+        <v>0</v>
+      </c>
       <c r="F17" s="3">
-        <f t="shared" ref="F17:V17" si="10">F7*25/96750</f>
-        <v>35.70542635658915</v>
+        <f>F8*10/96750</f>
+        <v>14.28217054263566</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="10"/>
-        <v>39.549354005167956</v>
+        <f>G8*10/96750</f>
+        <v>15.819741602067184</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="10"/>
-        <v>43.887080103359175</v>
+        <f>H8*10/96750</f>
+        <v>17.554832041343669</v>
       </c>
       <c r="I17" s="3">
-        <f t="shared" si="10"/>
-        <v>48.116279069767444</v>
-      </c>
-      <c r="J17" s="38">
-        <f t="shared" si="10"/>
-        <v>52.788888888888891</v>
-      </c>
-      <c r="K17" s="38">
-        <f t="shared" si="10"/>
-        <v>57.34780361757106</v>
-      </c>
-      <c r="L17" s="38">
-        <f t="shared" si="10"/>
-        <v>61.935400516795866</v>
-      </c>
-      <c r="M17" s="38">
-        <f t="shared" si="10"/>
-        <v>66.019896640826872</v>
-      </c>
-      <c r="N17" s="3">
-        <f t="shared" si="10"/>
-        <v>70.76614987080103</v>
-      </c>
-      <c r="O17" s="3">
-        <f t="shared" si="10"/>
-        <v>78.99483204134367</v>
-      </c>
-      <c r="P17" s="37">
-        <f t="shared" si="10"/>
-        <v>87.000258397932811</v>
-      </c>
-      <c r="Q17" s="3">
-        <f t="shared" si="10"/>
-        <v>94.830281653746766</v>
-      </c>
-      <c r="R17" s="3">
-        <f t="shared" si="10"/>
-        <v>103.87596899224806</v>
-      </c>
-      <c r="S17" s="3">
-        <f t="shared" si="10"/>
-        <v>113.22480620155041</v>
-      </c>
-      <c r="T17" s="3">
-        <f t="shared" si="10"/>
-        <v>123.41503875968993</v>
-      </c>
-      <c r="U17" s="3">
-        <f t="shared" si="10"/>
-        <v>134.52239224806203</v>
-      </c>
-      <c r="V17" s="3">
-        <f t="shared" si="10"/>
-        <v>146.62940755038764</v>
+        <f>I8*10/96750</f>
+        <v>19.246511627906976</v>
+      </c>
+      <c r="J17" s="3">
+        <f>J8*10/96750</f>
+        <v>21.115555555555556</v>
+      </c>
+      <c r="K17" s="3">
+        <f>K8*10/96750</f>
+        <v>22.939121447028423</v>
+      </c>
+      <c r="L17" s="3">
+        <f>L8*10/96750</f>
+        <v>24.774160206718346</v>
+      </c>
+      <c r="M17" s="12">
+        <f>M8*10/96750</f>
+        <v>26.407958656330749</v>
+      </c>
+      <c r="N17" s="38">
+        <f>N8*10/96750</f>
+        <v>28.306459948320413</v>
+      </c>
+      <c r="O17" s="38">
+        <f>O8*10/96750</f>
+        <v>31.597932816537469</v>
+      </c>
+      <c r="P17" s="35">
+        <f>P8*10/96750</f>
+        <v>34.800103359173129</v>
+      </c>
+      <c r="Q17" s="12">
+        <f>Q8*10/96750</f>
+        <v>37.911639513206495</v>
+      </c>
+      <c r="R17" s="12">
+        <f>R8*10/96750</f>
+        <v>41.550387596899228</v>
+      </c>
+      <c r="S17" s="12">
+        <f>S8*10/96750</f>
+        <v>45.184859475758209</v>
+      </c>
+      <c r="T17" s="12">
+        <f>T8*10/96750</f>
+        <v>49.143514204284315</v>
+      </c>
+      <c r="U17" s="12">
+        <f>U8*10/96750</f>
+        <v>53.49576085337285</v>
+      </c>
+      <c r="V17" s="12">
+        <f>V8*10/96750</f>
+        <v>58.384672153708124</v>
       </c>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="18" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3">
-        <f t="shared" ref="F18:V18" si="11">F7*30/96750</f>
-        <v>42.846511627906978</v>
+        <f>F8*12.5/96750</f>
+        <v>17.852713178294575</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="11"/>
-        <v>47.459224806201547</v>
-      </c>
-      <c r="H18" s="38">
-        <f t="shared" si="11"/>
-        <v>52.664496124031011</v>
-      </c>
-      <c r="I18" s="38">
-        <f t="shared" si="11"/>
-        <v>57.739534883720928</v>
-      </c>
-      <c r="J18" s="38">
-        <f t="shared" si="11"/>
-        <v>63.346666666666664</v>
-      </c>
-      <c r="K18" s="38">
-        <f t="shared" si="11"/>
-        <v>68.817364341085266</v>
-      </c>
-      <c r="L18" s="38">
-        <f t="shared" si="11"/>
-        <v>74.322480620155034</v>
-      </c>
-      <c r="M18" s="3">
-        <f t="shared" si="11"/>
-        <v>79.223875968992246</v>
-      </c>
-      <c r="N18" s="3">
-        <f t="shared" si="11"/>
-        <v>84.919379844961242</v>
-      </c>
-      <c r="O18" s="3">
-        <f t="shared" si="11"/>
-        <v>94.79379844961241</v>
+        <f>G8*12.5/96750</f>
+        <v>19.774677002583978</v>
+      </c>
+      <c r="H18" s="3">
+        <f>H8*12.5/96750</f>
+        <v>21.943540051679587</v>
+      </c>
+      <c r="I18" s="3">
+        <f>I8*12.5/96750</f>
+        <v>24.058139534883722</v>
+      </c>
+      <c r="J18" s="3">
+        <f>J8*12.5/96750</f>
+        <v>26.394444444444446</v>
+      </c>
+      <c r="K18" s="3">
+        <f>K8*12.5/96750</f>
+        <v>28.67390180878553</v>
+      </c>
+      <c r="L18" s="3">
+        <f>L8*12.5/96750</f>
+        <v>30.967700258397933</v>
+      </c>
+      <c r="M18" s="38">
+        <f>M8*12.5/96750</f>
+        <v>33.009948320413436</v>
+      </c>
+      <c r="N18" s="38">
+        <f>N8*12.5/96750</f>
+        <v>35.383074935400515</v>
+      </c>
+      <c r="O18" s="38">
+        <f>O8*12.5/96750</f>
+        <v>39.497416020671835</v>
       </c>
       <c r="P18" s="37">
-        <f t="shared" si="11"/>
-        <v>104.40031007751938</v>
+        <f>P8*12.5/96750</f>
+        <v>43.500129198966405</v>
       </c>
       <c r="Q18" s="3">
-        <f t="shared" si="11"/>
-        <v>113.79633798449612</v>
+        <f>Q8*12.5/96750</f>
+        <v>47.389549391508119</v>
       </c>
       <c r="R18" s="3">
-        <f t="shared" si="11"/>
-        <v>124.65116279069767</v>
+        <f>R8*12.5/96750</f>
+        <v>51.937984496124031</v>
       </c>
       <c r="S18" s="3">
-        <f t="shared" si="11"/>
-        <v>135.86976744186049</v>
+        <f>S8*12.5/96750</f>
+        <v>56.48107434469776</v>
       </c>
       <c r="T18" s="3">
-        <f t="shared" si="11"/>
-        <v>148.09804651162793</v>
+        <f>T8*12.5/96750</f>
+        <v>61.429392755355387</v>
       </c>
       <c r="U18" s="3">
-        <f t="shared" si="11"/>
-        <v>161.42687069767445</v>
+        <f>U8*12.5/96750</f>
+        <v>66.869701066716075</v>
       </c>
       <c r="V18" s="3">
-        <f t="shared" si="11"/>
-        <v>175.95528906046516</v>
+        <f>V8*12.5/96750</f>
+        <v>72.980840192135162</v>
       </c>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="18" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="D19" s="3">
+        <f>D8*15/96750</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <f>E8*15/96750</f>
+        <v>0</v>
+      </c>
       <c r="F19" s="3">
-        <f t="shared" ref="F19:V19" si="12">F7*40/96750</f>
-        <v>57.128682170542639</v>
-      </c>
-      <c r="G19" s="38">
-        <f t="shared" si="12"/>
-        <v>63.278966408268737</v>
-      </c>
-      <c r="H19" s="38">
-        <f t="shared" si="12"/>
-        <v>70.219328165374677</v>
-      </c>
-      <c r="I19" s="38">
-        <f t="shared" si="12"/>
-        <v>76.986046511627904</v>
-      </c>
-      <c r="J19" s="38">
-        <f t="shared" si="12"/>
-        <v>84.462222222222223</v>
+        <f>F8*15/96750</f>
+        <v>21.423255813953489</v>
+      </c>
+      <c r="G19" s="3">
+        <f>G8*15/96750</f>
+        <v>23.729612403100774</v>
+      </c>
+      <c r="H19" s="3">
+        <f>H8*15/96750</f>
+        <v>26.332248062015505</v>
+      </c>
+      <c r="I19" s="3">
+        <f>I8*15/96750</f>
+        <v>28.869767441860464</v>
+      </c>
+      <c r="J19" s="3">
+        <f>J8*15/96750</f>
+        <v>31.673333333333332</v>
       </c>
       <c r="K19" s="3">
-        <f t="shared" si="12"/>
-        <v>91.756485788113693</v>
-      </c>
-      <c r="L19" s="38">
-        <f t="shared" si="12"/>
-        <v>99.096640826873383</v>
-      </c>
-      <c r="M19" s="3">
-        <f t="shared" si="12"/>
-        <v>105.63183462532299</v>
-      </c>
-      <c r="N19" s="3">
-        <f t="shared" si="12"/>
-        <v>113.22583979328165</v>
-      </c>
-      <c r="O19" s="3">
-        <f t="shared" si="12"/>
-        <v>126.39173126614988</v>
-      </c>
-      <c r="P19" s="37">
-        <f t="shared" si="12"/>
-        <v>139.20041343669251</v>
-      </c>
-      <c r="Q19" s="3">
-        <f t="shared" si="12"/>
-        <v>151.72845064599483</v>
-      </c>
-      <c r="R19" s="3">
-        <f t="shared" si="12"/>
-        <v>166.20155038759691</v>
-      </c>
-      <c r="S19" s="3">
-        <f t="shared" si="12"/>
-        <v>181.15968992248065</v>
-      </c>
-      <c r="T19" s="3">
-        <f t="shared" si="12"/>
-        <v>197.46406201550391</v>
-      </c>
-      <c r="U19" s="3">
-        <f t="shared" si="12"/>
-        <v>215.23582759689927</v>
-      </c>
-      <c r="V19" s="3">
-        <f t="shared" si="12"/>
-        <v>234.60705208062024</v>
+        <f>K8*15/96750</f>
+        <v>34.408682170542633</v>
+      </c>
+      <c r="L19" s="3">
+        <f>L8*15/96750</f>
+        <v>37.161240310077517</v>
+      </c>
+      <c r="M19" s="38">
+        <f>M8*15/96750</f>
+        <v>39.611937984496123</v>
+      </c>
+      <c r="N19" s="38">
+        <f>N8*15/96750</f>
+        <v>42.459689922480621</v>
+      </c>
+      <c r="O19" s="12">
+        <f>O8*15/96750</f>
+        <v>47.396899224806205</v>
+      </c>
+      <c r="P19" s="35">
+        <f>P8*15/96750</f>
+        <v>52.200155038759689</v>
+      </c>
+      <c r="Q19" s="12">
+        <f>Q8*15/96750</f>
+        <v>56.867459269809743</v>
+      </c>
+      <c r="R19" s="12">
+        <f>R8*15/96750</f>
+        <v>62.325581395348834</v>
+      </c>
+      <c r="S19" s="12">
+        <f>S8*15/96750</f>
+        <v>67.777289213637303</v>
+      </c>
+      <c r="T19" s="12">
+        <f>T8*15/96750</f>
+        <v>73.715271306426473</v>
+      </c>
+      <c r="U19" s="12">
+        <f>U8*15/96750</f>
+        <v>80.243641280059279</v>
+      </c>
+      <c r="V19" s="12">
+        <f>V8*15/96750</f>
+        <v>87.577008230562186</v>
       </c>
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="18" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3">
-        <f t="shared" ref="F20:V20" si="13">F7*50/96750</f>
-        <v>71.410852713178301</v>
-      </c>
-      <c r="G20" s="38">
-        <f t="shared" si="13"/>
-        <v>79.098708010335912</v>
-      </c>
-      <c r="H20" s="38">
-        <f t="shared" si="13"/>
-        <v>87.774160206718349</v>
-      </c>
-      <c r="I20" s="38">
-        <f t="shared" si="13"/>
-        <v>96.232558139534888</v>
-      </c>
-      <c r="J20" s="3">
-        <f t="shared" si="13"/>
-        <v>105.57777777777778</v>
+        <f>F8*17.5/96750</f>
+        <v>24.993798449612402</v>
+      </c>
+      <c r="G20" s="3">
+        <f>G8*17.5/96750</f>
+        <v>27.684547803617573</v>
+      </c>
+      <c r="H20" s="3">
+        <f>H8*17.5/96750</f>
+        <v>30.72095607235142</v>
+      </c>
+      <c r="I20" s="3">
+        <f>I8*17.5/96750</f>
+        <v>33.681395348837206</v>
+      </c>
+      <c r="J20" s="38">
+        <f>J8*17.5/96750</f>
+        <v>36.952222222222225</v>
       </c>
       <c r="K20" s="3">
-        <f t="shared" si="13"/>
-        <v>114.69560723514212</v>
+        <f>K8*17.5/96750</f>
+        <v>40.143462532299743</v>
       </c>
       <c r="L20" s="3">
-        <f t="shared" si="13"/>
-        <v>123.87080103359173</v>
-      </c>
-      <c r="M20" s="3">
-        <f t="shared" si="13"/>
-        <v>132.03979328165374</v>
+        <f>L8*17.5/96750</f>
+        <v>43.354780361757108</v>
+      </c>
+      <c r="M20" s="38">
+        <f>M8*17.5/96750</f>
+        <v>46.21392764857881</v>
       </c>
       <c r="N20" s="3">
-        <f t="shared" si="13"/>
-        <v>141.53229974160206</v>
+        <f>N8*17.5/96750</f>
+        <v>49.536304909560727</v>
       </c>
       <c r="O20" s="3">
-        <f t="shared" si="13"/>
-        <v>157.98966408268734</v>
+        <f>O8*17.5/96750</f>
+        <v>55.296382428940568</v>
       </c>
       <c r="P20" s="37">
-        <f t="shared" si="13"/>
-        <v>174.00051679586562</v>
+        <f>P8*17.5/96750</f>
+        <v>60.900180878552973</v>
       </c>
       <c r="Q20" s="3">
-        <f t="shared" si="13"/>
-        <v>189.66056330749353</v>
+        <f>Q8*17.5/96750</f>
+        <v>66.345369148111374</v>
       </c>
       <c r="R20" s="3">
-        <f t="shared" si="13"/>
-        <v>207.75193798449612</v>
+        <f>R8*17.5/96750</f>
+        <v>72.713178294573638</v>
       </c>
       <c r="S20" s="3">
-        <f t="shared" si="13"/>
-        <v>226.44961240310082</v>
+        <f>S8*17.5/96750</f>
+        <v>79.073504082576861</v>
       </c>
       <c r="T20" s="3">
-        <f t="shared" si="13"/>
-        <v>246.83007751937987</v>
+        <f>T8*17.5/96750</f>
+        <v>86.001149857497552</v>
       </c>
       <c r="U20" s="3">
-        <f t="shared" si="13"/>
-        <v>269.04478449612407</v>
+        <f>U8*17.5/96750</f>
+        <v>93.617581493402497</v>
       </c>
       <c r="V20" s="3">
-        <f t="shared" si="13"/>
-        <v>293.25881510077528</v>
+        <f>V8*17.5/96750</f>
+        <v>102.17317626898922</v>
       </c>
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="18" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="D21" s="3">
+        <f>D8*20/96750</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <f>E8*20/96750</f>
+        <v>0</v>
+      </c>
       <c r="F21" s="3">
-        <f t="shared" ref="F21:V21" si="14">F7*60/96750</f>
-        <v>85.693023255813955</v>
-      </c>
-      <c r="G21" s="38">
-        <f t="shared" si="14"/>
-        <v>94.918449612403094</v>
-      </c>
-      <c r="H21" s="38">
-        <f t="shared" si="14"/>
-        <v>105.32899224806202</v>
+        <f>F8*20/96750</f>
+        <v>28.56434108527132</v>
+      </c>
+      <c r="G21" s="3">
+        <f>G8*20/96750</f>
+        <v>31.639483204134368</v>
+      </c>
+      <c r="H21" s="3">
+        <f>H8*20/96750</f>
+        <v>35.109664082687338</v>
       </c>
       <c r="I21" s="3">
-        <f t="shared" si="14"/>
-        <v>115.47906976744186</v>
-      </c>
-      <c r="J21" s="3">
-        <f t="shared" si="14"/>
-        <v>126.69333333333333</v>
+        <f>I8*20/96750</f>
+        <v>38.493023255813952</v>
+      </c>
+      <c r="J21" s="38">
+        <f>J8*20/96750</f>
+        <v>42.231111111111112</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="14"/>
-        <v>137.63472868217053</v>
-      </c>
-      <c r="L21" s="3">
-        <f t="shared" si="14"/>
-        <v>148.64496124031007</v>
-      </c>
-      <c r="M21" s="3">
-        <f t="shared" si="14"/>
-        <v>158.44775193798449</v>
+        <f>K8*20/96750</f>
+        <v>45.878242894056847</v>
+      </c>
+      <c r="L21" s="38">
+        <f>L8*20/96750</f>
+        <v>49.548320413436691</v>
+      </c>
+      <c r="M21" s="38">
+        <f>M8*20/96750</f>
+        <v>52.815917312661497</v>
       </c>
       <c r="N21" s="3">
-        <f t="shared" si="14"/>
-        <v>169.83875968992248</v>
-      </c>
-      <c r="O21" s="3">
-        <f t="shared" si="14"/>
-        <v>189.58759689922482</v>
-      </c>
-      <c r="P21" s="37">
-        <f t="shared" si="14"/>
-        <v>208.80062015503876</v>
-      </c>
-      <c r="Q21" s="3">
-        <f t="shared" si="14"/>
-        <v>227.59267596899224</v>
-      </c>
-      <c r="R21" s="3">
-        <f t="shared" si="14"/>
-        <v>249.30232558139534</v>
-      </c>
-      <c r="S21" s="3">
-        <f t="shared" si="14"/>
-        <v>271.73953488372098</v>
-      </c>
-      <c r="T21" s="3">
-        <f t="shared" si="14"/>
-        <v>296.19609302325586</v>
-      </c>
-      <c r="U21" s="3">
-        <f t="shared" si="14"/>
-        <v>322.85374139534889</v>
-      </c>
-      <c r="V21" s="3">
-        <f t="shared" si="14"/>
-        <v>351.91057812093032</v>
+        <f>N8*20/96750</f>
+        <v>56.612919896640825</v>
+      </c>
+      <c r="O21" s="12">
+        <f>O8*20/96750</f>
+        <v>63.195865633074938</v>
+      </c>
+      <c r="P21" s="35">
+        <f>P8*20/96750</f>
+        <v>69.600206718346257</v>
+      </c>
+      <c r="Q21" s="12">
+        <f>Q8*20/96750</f>
+        <v>75.82327902641299</v>
+      </c>
+      <c r="R21" s="12">
+        <f>R8*20/96750</f>
+        <v>83.100775193798455</v>
+      </c>
+      <c r="S21" s="12">
+        <f>S8*20/96750</f>
+        <v>90.369718951516418</v>
+      </c>
+      <c r="T21" s="12">
+        <f>T8*20/96750</f>
+        <v>98.287028408568631</v>
+      </c>
+      <c r="U21" s="12">
+        <f>U8*20/96750</f>
+        <v>106.9915217067457</v>
+      </c>
+      <c r="V21" s="12">
+        <f>V8*20/96750</f>
+        <v>116.76934430741625</v>
       </c>
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="18" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3">
-        <f t="shared" ref="F22:V22" si="15">F7*70/96750</f>
-        <v>99.97519379844961</v>
-      </c>
-      <c r="G22" s="38">
-        <f t="shared" si="15"/>
-        <v>110.73819121447029</v>
+        <f>F8*25/96750</f>
+        <v>35.70542635658915</v>
+      </c>
+      <c r="G22" s="3">
+        <f>G8*25/96750</f>
+        <v>39.549354005167956</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="15"/>
-        <v>122.88382428940568</v>
+        <f>H8*25/96750</f>
+        <v>43.887080103359175</v>
       </c>
       <c r="I22" s="3">
-        <f t="shared" si="15"/>
-        <v>134.72558139534883</v>
-      </c>
-      <c r="J22" s="3">
-        <f t="shared" si="15"/>
-        <v>147.8088888888889</v>
-      </c>
-      <c r="K22" s="3">
-        <f t="shared" si="15"/>
-        <v>160.57385012919897</v>
-      </c>
-      <c r="L22" s="3">
-        <f t="shared" si="15"/>
-        <v>173.41912144702843</v>
-      </c>
-      <c r="M22" s="3">
-        <f t="shared" si="15"/>
-        <v>184.85571059431524</v>
+        <f>I8*25/96750</f>
+        <v>48.116279069767444</v>
+      </c>
+      <c r="J22" s="38">
+        <f>J8*25/96750</f>
+        <v>52.788888888888891</v>
+      </c>
+      <c r="K22" s="38">
+        <f>K8*25/96750</f>
+        <v>57.34780361757106</v>
+      </c>
+      <c r="L22" s="38">
+        <f>L8*25/96750</f>
+        <v>61.935400516795866</v>
+      </c>
+      <c r="M22" s="38">
+        <f>M8*25/96750</f>
+        <v>66.019896640826872</v>
       </c>
       <c r="N22" s="3">
-        <f t="shared" si="15"/>
-        <v>198.14521963824291</v>
+        <f>N8*25/96750</f>
+        <v>70.76614987080103</v>
       </c>
       <c r="O22" s="3">
-        <f t="shared" si="15"/>
-        <v>221.18552971576227</v>
+        <f>O8*25/96750</f>
+        <v>78.99483204134367</v>
       </c>
       <c r="P22" s="37">
-        <f t="shared" si="15"/>
-        <v>243.60072351421189</v>
+        <f>P8*25/96750</f>
+        <v>87.000258397932811</v>
       </c>
       <c r="Q22" s="3">
-        <f t="shared" si="15"/>
-        <v>265.52478863049095</v>
+        <f>Q8*25/96750</f>
+        <v>94.779098783016238</v>
       </c>
       <c r="R22" s="3">
-        <f t="shared" si="15"/>
-        <v>290.85271317829455</v>
+        <f>R8*25/96750</f>
+        <v>103.87596899224806</v>
       </c>
       <c r="S22" s="3">
-        <f t="shared" si="15"/>
-        <v>317.02945736434111</v>
+        <f>S8*25/96750</f>
+        <v>112.96214868939552</v>
       </c>
       <c r="T22" s="3">
-        <f t="shared" si="15"/>
-        <v>345.56210852713184</v>
+        <f>T8*25/96750</f>
+        <v>122.85878551071077</v>
       </c>
       <c r="U22" s="3">
-        <f t="shared" si="15"/>
-        <v>376.66269829457377</v>
+        <f>U8*25/96750</f>
+        <v>133.73940213343215</v>
       </c>
       <c r="V22" s="3">
-        <f t="shared" si="15"/>
-        <v>410.56234114108543</v>
+        <f>V8*25/96750</f>
+        <v>145.96168038427032</v>
       </c>
     </row>
     <row r="23" spans="1:22">
-      <c r="A23" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40">
-        <f t="shared" ref="F23:V23" si="16">F7*80/96750</f>
-        <v>114.25736434108528</v>
-      </c>
-      <c r="G23" s="40">
-        <f t="shared" si="16"/>
-        <v>126.55793281653747</v>
-      </c>
-      <c r="H23" s="40">
-        <f t="shared" si="16"/>
-        <v>140.43865633074935</v>
-      </c>
-      <c r="I23" s="40">
-        <f t="shared" si="16"/>
-        <v>153.97209302325581</v>
-      </c>
-      <c r="J23" s="40">
-        <f t="shared" si="16"/>
-        <v>168.92444444444445</v>
-      </c>
-      <c r="K23" s="40">
-        <f t="shared" si="16"/>
-        <v>183.51297157622739</v>
-      </c>
-      <c r="L23" s="40">
-        <f t="shared" si="16"/>
-        <v>198.19328165374677</v>
-      </c>
-      <c r="M23" s="40">
-        <f t="shared" si="16"/>
-        <v>211.26366925064599</v>
-      </c>
-      <c r="N23" s="40">
-        <f t="shared" si="16"/>
-        <v>226.4516795865633</v>
-      </c>
-      <c r="O23" s="40">
-        <f t="shared" si="16"/>
-        <v>252.78346253229975</v>
-      </c>
-      <c r="P23" s="41">
-        <f t="shared" si="16"/>
-        <v>278.40082687338503</v>
-      </c>
-      <c r="Q23" s="40">
-        <f t="shared" si="16"/>
-        <v>303.45690129198965</v>
-      </c>
-      <c r="R23" s="40">
-        <f t="shared" si="16"/>
-        <v>332.40310077519382</v>
-      </c>
-      <c r="S23" s="40">
-        <f t="shared" si="16"/>
-        <v>362.3193798449613</v>
-      </c>
-      <c r="T23" s="40">
-        <f t="shared" si="16"/>
-        <v>394.92812403100783</v>
-      </c>
-      <c r="U23" s="40">
-        <f t="shared" si="16"/>
-        <v>430.47165519379854</v>
-      </c>
-      <c r="V23" s="40">
-        <f t="shared" si="16"/>
-        <v>469.21410416124047</v>
+      <c r="A23" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3">
+        <f>F8*30/96750</f>
+        <v>42.846511627906978</v>
+      </c>
+      <c r="G23" s="3">
+        <f>G8*30/96750</f>
+        <v>47.459224806201547</v>
+      </c>
+      <c r="H23" s="38">
+        <f>H8*30/96750</f>
+        <v>52.664496124031011</v>
+      </c>
+      <c r="I23" s="38">
+        <f>I8*30/96750</f>
+        <v>57.739534883720928</v>
+      </c>
+      <c r="J23" s="38">
+        <f>J8*30/96750</f>
+        <v>63.346666666666664</v>
+      </c>
+      <c r="K23" s="38">
+        <f>K8*30/96750</f>
+        <v>68.817364341085266</v>
+      </c>
+      <c r="L23" s="38">
+        <f>L8*30/96750</f>
+        <v>74.322480620155034</v>
+      </c>
+      <c r="M23" s="3">
+        <f>M8*30/96750</f>
+        <v>79.223875968992246</v>
+      </c>
+      <c r="N23" s="3">
+        <f>N8*30/96750</f>
+        <v>84.919379844961242</v>
+      </c>
+      <c r="O23" s="3">
+        <f>O8*30/96750</f>
+        <v>94.79379844961241</v>
+      </c>
+      <c r="P23" s="37">
+        <f>P8*30/96750</f>
+        <v>104.40031007751938</v>
+      </c>
+      <c r="Q23" s="3">
+        <f>Q8*30/96750</f>
+        <v>113.73491853961949</v>
+      </c>
+      <c r="R23" s="3">
+        <f>R8*30/96750</f>
+        <v>124.65116279069767</v>
+      </c>
+      <c r="S23" s="3">
+        <f>S8*30/96750</f>
+        <v>135.55457842727461</v>
+      </c>
+      <c r="T23" s="3">
+        <f>T8*30/96750</f>
+        <v>147.43054261285295</v>
+      </c>
+      <c r="U23" s="3">
+        <f>U8*30/96750</f>
+        <v>160.48728256011856</v>
+      </c>
+      <c r="V23" s="3">
+        <f>V8*30/96750</f>
+        <v>175.15401646112437</v>
       </c>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="3"/>
+      <c r="A24" s="18" t="s">
+        <v>160</v>
+      </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="12"/>
-      <c r="S24" s="12"/>
-      <c r="T24" s="12"/>
-      <c r="U24" s="12"/>
-      <c r="V24" s="12"/>
+      <c r="F24" s="3">
+        <f>F8*40/96750</f>
+        <v>57.128682170542639</v>
+      </c>
+      <c r="G24" s="38">
+        <f>G8*40/96750</f>
+        <v>63.278966408268737</v>
+      </c>
+      <c r="H24" s="38">
+        <f>H8*40/96750</f>
+        <v>70.219328165374677</v>
+      </c>
+      <c r="I24" s="38">
+        <f>I8*40/96750</f>
+        <v>76.986046511627904</v>
+      </c>
+      <c r="J24" s="38">
+        <f>J8*40/96750</f>
+        <v>84.462222222222223</v>
+      </c>
+      <c r="K24" s="3">
+        <f>K8*40/96750</f>
+        <v>91.756485788113693</v>
+      </c>
+      <c r="L24" s="38">
+        <f>L8*40/96750</f>
+        <v>99.096640826873383</v>
+      </c>
+      <c r="M24" s="3">
+        <f>M8*40/96750</f>
+        <v>105.63183462532299</v>
+      </c>
+      <c r="N24" s="3">
+        <f>N8*40/96750</f>
+        <v>113.22583979328165</v>
+      </c>
+      <c r="O24" s="3">
+        <f>O8*40/96750</f>
+        <v>126.39173126614988</v>
+      </c>
+      <c r="P24" s="37">
+        <f>P8*40/96750</f>
+        <v>139.20041343669251</v>
+      </c>
+      <c r="Q24" s="3">
+        <f>Q8*40/96750</f>
+        <v>151.64655805282598</v>
+      </c>
+      <c r="R24" s="3">
+        <f>R8*40/96750</f>
+        <v>166.20155038759691</v>
+      </c>
+      <c r="S24" s="3">
+        <f>S8*40/96750</f>
+        <v>180.73943790303284</v>
+      </c>
+      <c r="T24" s="3">
+        <f>T8*40/96750</f>
+        <v>196.57405681713726</v>
+      </c>
+      <c r="U24" s="3">
+        <f>U8*40/96750</f>
+        <v>213.9830434134914</v>
+      </c>
+      <c r="V24" s="3">
+        <f>V8*40/96750</f>
+        <v>233.53868861483249</v>
+      </c>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="3" t="s">
-        <v>165</v>
+      <c r="A25" s="18" t="s">
+        <v>161</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="12"/>
-      <c r="S25" s="12"/>
-      <c r="T25" s="12"/>
-      <c r="U25" s="12"/>
-      <c r="V25" s="12"/>
+      <c r="F25" s="3">
+        <f>F8*50/96750</f>
+        <v>71.410852713178301</v>
+      </c>
+      <c r="G25" s="38">
+        <f>G8*50/96750</f>
+        <v>79.098708010335912</v>
+      </c>
+      <c r="H25" s="38">
+        <f>H8*50/96750</f>
+        <v>87.774160206718349</v>
+      </c>
+      <c r="I25" s="38">
+        <f>I8*50/96750</f>
+        <v>96.232558139534888</v>
+      </c>
+      <c r="J25" s="3">
+        <f>J8*50/96750</f>
+        <v>105.57777777777778</v>
+      </c>
+      <c r="K25" s="3">
+        <f>K8*50/96750</f>
+        <v>114.69560723514212</v>
+      </c>
+      <c r="L25" s="3">
+        <f>L8*50/96750</f>
+        <v>123.87080103359173</v>
+      </c>
+      <c r="M25" s="3">
+        <f>M8*50/96750</f>
+        <v>132.03979328165374</v>
+      </c>
+      <c r="N25" s="3">
+        <f>N8*50/96750</f>
+        <v>141.53229974160206</v>
+      </c>
+      <c r="O25" s="3">
+        <f>O8*50/96750</f>
+        <v>157.98966408268734</v>
+      </c>
+      <c r="P25" s="37">
+        <f>P8*50/96750</f>
+        <v>174.00051679586562</v>
+      </c>
+      <c r="Q25" s="3">
+        <f>Q8*50/96750</f>
+        <v>189.55819756603248</v>
+      </c>
+      <c r="R25" s="3">
+        <f>R8*50/96750</f>
+        <v>207.75193798449612</v>
+      </c>
+      <c r="S25" s="3">
+        <f>S8*50/96750</f>
+        <v>225.92429737879104</v>
+      </c>
+      <c r="T25" s="3">
+        <f>T8*50/96750</f>
+        <v>245.71757102142155</v>
+      </c>
+      <c r="U25" s="3">
+        <f>U8*50/96750</f>
+        <v>267.4788042668643</v>
+      </c>
+      <c r="V25" s="3">
+        <f>V8*50/96750</f>
+        <v>291.92336076854065</v>
+      </c>
     </row>
     <row r="26" spans="1:22">
-      <c r="A26" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" s="42" t="str">
-        <f t="shared" ref="B26:V26" si="17">B3</f>
-        <v>Actual</v>
-      </c>
-      <c r="C26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="D26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="E26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="F26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="G26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="H26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="I26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="J26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="K26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="L26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="M26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="N26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="O26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Actual</v>
-      </c>
-      <c r="P26" s="43" t="str">
-        <f t="shared" si="17"/>
-        <v>Guidance:</v>
-      </c>
-      <c r="Q26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Estimated</v>
-      </c>
-      <c r="R26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Estimated</v>
-      </c>
-      <c r="S26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Estimated</v>
-      </c>
-      <c r="T26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Estimated</v>
-      </c>
-      <c r="U26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Estimated</v>
-      </c>
-      <c r="V26" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>Estimated</v>
+      <c r="A26" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <f>F8*60/96750</f>
+        <v>85.693023255813955</v>
+      </c>
+      <c r="G26" s="38">
+        <f>G8*60/96750</f>
+        <v>94.918449612403094</v>
+      </c>
+      <c r="H26" s="38">
+        <f>H8*60/96750</f>
+        <v>105.32899224806202</v>
+      </c>
+      <c r="I26" s="3">
+        <f>I8*60/96750</f>
+        <v>115.47906976744186</v>
+      </c>
+      <c r="J26" s="3">
+        <f>J8*60/96750</f>
+        <v>126.69333333333333</v>
+      </c>
+      <c r="K26" s="3">
+        <f>K8*60/96750</f>
+        <v>137.63472868217053</v>
+      </c>
+      <c r="L26" s="3">
+        <f>L8*60/96750</f>
+        <v>148.64496124031007</v>
+      </c>
+      <c r="M26" s="3">
+        <f>M8*60/96750</f>
+        <v>158.44775193798449</v>
+      </c>
+      <c r="N26" s="3">
+        <f>N8*60/96750</f>
+        <v>169.83875968992248</v>
+      </c>
+      <c r="O26" s="3">
+        <f>O8*60/96750</f>
+        <v>189.58759689922482</v>
+      </c>
+      <c r="P26" s="37">
+        <f>P8*60/96750</f>
+        <v>208.80062015503876</v>
+      </c>
+      <c r="Q26" s="3">
+        <f>Q8*60/96750</f>
+        <v>227.46983707923897</v>
+      </c>
+      <c r="R26" s="3">
+        <f>R8*60/96750</f>
+        <v>249.30232558139534</v>
+      </c>
+      <c r="S26" s="3">
+        <f>S8*60/96750</f>
+        <v>271.10915685454921</v>
+      </c>
+      <c r="T26" s="3">
+        <f>T8*60/96750</f>
+        <v>294.86108522570589</v>
+      </c>
+      <c r="U26" s="3">
+        <f>U8*60/96750</f>
+        <v>320.97456512023712</v>
+      </c>
+      <c r="V26" s="3">
+        <f>V8*60/96750</f>
+        <v>350.30803292224874</v>
       </c>
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B27" s="3" t="str">
-        <f t="shared" ref="B27:V27" si="18">B4</f>
-        <v>Q4 FY 19</v>
-      </c>
-      <c r="C27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q1 FY 20</v>
-      </c>
-      <c r="D27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q2 FY 20</v>
-      </c>
-      <c r="E27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q3 FY 20</v>
-      </c>
-      <c r="F27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q4 FY 20</v>
-      </c>
-      <c r="G27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q1 FY 21</v>
-      </c>
-      <c r="H27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q2 FY 21</v>
-      </c>
-      <c r="I27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q3 FY 21</v>
-      </c>
-      <c r="J27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q4 FY 21</v>
-      </c>
-      <c r="K27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q1 FY 22</v>
-      </c>
-      <c r="L27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q2 FY 22</v>
-      </c>
-      <c r="M27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q3 FY 22</v>
-      </c>
-      <c r="N27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q4 FY 22</v>
-      </c>
-      <c r="O27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q1 FY 23</v>
-      </c>
-      <c r="P27" s="37" t="str">
-        <f t="shared" si="18"/>
-        <v>Q2 FY 23</v>
-      </c>
-      <c r="Q27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q3 FY 23</v>
-      </c>
-      <c r="R27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q4 FY 23</v>
-      </c>
-      <c r="S27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q1 FY 24</v>
-      </c>
-      <c r="T27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q2 FY 24</v>
-      </c>
-      <c r="U27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q3 FY 24</v>
-      </c>
-      <c r="V27" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>Q4 FY 24</v>
+        <v>163</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3">
+        <f>F8*70/96750</f>
+        <v>99.97519379844961</v>
+      </c>
+      <c r="G27" s="38">
+        <f>G8*70/96750</f>
+        <v>110.73819121447029</v>
+      </c>
+      <c r="H27" s="3">
+        <f>H8*70/96750</f>
+        <v>122.88382428940568</v>
+      </c>
+      <c r="I27" s="3">
+        <f>I8*70/96750</f>
+        <v>134.72558139534883</v>
+      </c>
+      <c r="J27" s="3">
+        <f>J8*70/96750</f>
+        <v>147.8088888888889</v>
+      </c>
+      <c r="K27" s="3">
+        <f>K8*70/96750</f>
+        <v>160.57385012919897</v>
+      </c>
+      <c r="L27" s="3">
+        <f>L8*70/96750</f>
+        <v>173.41912144702843</v>
+      </c>
+      <c r="M27" s="3">
+        <f>M8*70/96750</f>
+        <v>184.85571059431524</v>
+      </c>
+      <c r="N27" s="3">
+        <f>N8*70/96750</f>
+        <v>198.14521963824291</v>
+      </c>
+      <c r="O27" s="3">
+        <f>O8*70/96750</f>
+        <v>221.18552971576227</v>
+      </c>
+      <c r="P27" s="37">
+        <f>P8*70/96750</f>
+        <v>243.60072351421189</v>
+      </c>
+      <c r="Q27" s="3">
+        <f>Q8*70/96750</f>
+        <v>265.38147659244549</v>
+      </c>
+      <c r="R27" s="3">
+        <f>R8*70/96750</f>
+        <v>290.85271317829455</v>
+      </c>
+      <c r="S27" s="3">
+        <f>S8*70/96750</f>
+        <v>316.29401633030744</v>
+      </c>
+      <c r="T27" s="3">
+        <f>T8*70/96750</f>
+        <v>344.00459942999021</v>
+      </c>
+      <c r="U27" s="3">
+        <f>U8*70/96750</f>
+        <v>374.47032597360999</v>
+      </c>
+      <c r="V27" s="3">
+        <f>V8*70/96750</f>
+        <v>408.69270507595689</v>
       </c>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="B28" s="44">
-        <f t="shared" ref="B28:V28" si="19">B5</f>
-        <v>43496</v>
-      </c>
-      <c r="C28" s="45">
-        <f t="shared" si="19"/>
-        <v>43585</v>
-      </c>
-      <c r="D28" s="44">
-        <f t="shared" si="19"/>
-        <v>43677</v>
-      </c>
-      <c r="E28" s="44">
-        <f t="shared" si="19"/>
-        <v>43769</v>
-      </c>
-      <c r="F28" s="44">
-        <f t="shared" si="19"/>
-        <v>43861</v>
-      </c>
-      <c r="G28" s="45">
-        <f t="shared" si="19"/>
-        <v>43951</v>
-      </c>
-      <c r="H28" s="44">
-        <f t="shared" si="19"/>
-        <v>44043</v>
-      </c>
-      <c r="I28" s="44">
-        <f t="shared" si="19"/>
-        <v>44135</v>
-      </c>
-      <c r="J28" s="44">
-        <f t="shared" si="19"/>
-        <v>44227</v>
-      </c>
-      <c r="K28" s="45">
-        <f t="shared" si="19"/>
-        <v>44316</v>
-      </c>
-      <c r="L28" s="44">
-        <f t="shared" si="19"/>
-        <v>44408</v>
-      </c>
-      <c r="M28" s="44">
-        <f t="shared" si="19"/>
-        <v>44500</v>
-      </c>
-      <c r="N28" s="44">
-        <f t="shared" si="19"/>
-        <v>44592</v>
-      </c>
-      <c r="O28" s="45">
-        <f t="shared" si="19"/>
-        <v>44681</v>
-      </c>
-      <c r="P28" s="46">
-        <f t="shared" si="19"/>
-        <v>44773</v>
-      </c>
-      <c r="Q28" s="44">
-        <f t="shared" si="19"/>
-        <v>44865</v>
-      </c>
-      <c r="R28" s="44">
-        <f t="shared" si="19"/>
-        <v>44957</v>
-      </c>
-      <c r="S28" s="45">
-        <f t="shared" si="19"/>
-        <v>45046</v>
-      </c>
-      <c r="T28" s="44">
-        <f t="shared" si="19"/>
-        <v>45138</v>
-      </c>
-      <c r="U28" s="44">
-        <f t="shared" si="19"/>
-        <v>45230</v>
-      </c>
-      <c r="V28" s="44">
-        <f t="shared" si="19"/>
-        <v>45322</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22">
-      <c r="A29" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="13">
-        <f t="shared" ref="C29:P29" si="20">C6</f>
-        <v>29836</v>
-      </c>
-      <c r="D29" s="13">
-        <f t="shared" si="20"/>
-        <v>31978</v>
-      </c>
-      <c r="E29" s="13">
-        <f t="shared" si="20"/>
-        <v>37862</v>
-      </c>
-      <c r="F29" s="13">
-        <f t="shared" si="20"/>
-        <v>38504</v>
-      </c>
-      <c r="G29" s="13">
-        <f t="shared" si="20"/>
-        <v>44712</v>
-      </c>
-      <c r="H29" s="13">
-        <f t="shared" si="20"/>
-        <v>48765</v>
-      </c>
-      <c r="I29" s="13">
-        <f t="shared" si="20"/>
-        <v>54229</v>
-      </c>
-      <c r="J29" s="13">
-        <f t="shared" si="20"/>
-        <v>56587</v>
-      </c>
-      <c r="K29" s="13">
-        <f t="shared" si="20"/>
-        <v>62355</v>
-      </c>
-      <c r="L29" s="13">
-        <f t="shared" si="20"/>
-        <v>66519</v>
-      </c>
-      <c r="M29" s="13">
-        <f t="shared" si="20"/>
-        <v>70036</v>
-      </c>
-      <c r="N29" s="13">
-        <f t="shared" si="20"/>
-        <v>74955</v>
-      </c>
-      <c r="O29" s="13">
-        <f t="shared" si="20"/>
-        <v>94200</v>
-      </c>
-      <c r="P29" s="47">
-        <f t="shared" si="20"/>
-        <v>97500</v>
-      </c>
-      <c r="Q29" s="29">
-        <f t="shared" ref="Q29:V29" si="21">Q31-SUM(N29:P29)</f>
-        <v>100338.19</v>
-      </c>
-      <c r="R29" s="29">
-        <f t="shared" si="21"/>
-        <v>109961.81</v>
-      </c>
-      <c r="S29" s="29">
-        <f t="shared" si="21"/>
-        <v>130380.00000000006</v>
-      </c>
-      <c r="T29" s="29">
-        <f t="shared" si="21"/>
-        <v>136936.20000000001</v>
-      </c>
-      <c r="U29" s="29">
-        <f t="shared" si="21"/>
-        <v>143323.64800000004</v>
-      </c>
-      <c r="V29" s="29">
-        <f t="shared" si="21"/>
-        <v>156815.95922000008</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22">
-      <c r="A30" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="48">
-        <f t="shared" ref="D30:V30" si="22">(D29-C29)/C29</f>
-        <v>7.1792465477946099E-2</v>
-      </c>
-      <c r="E30" s="48">
-        <f t="shared" si="22"/>
-        <v>0.18400150103195947</v>
-      </c>
-      <c r="F30" s="48">
-        <f t="shared" si="22"/>
-        <v>1.6956315038825207E-2</v>
-      </c>
-      <c r="G30" s="48">
-        <f t="shared" si="22"/>
-        <v>0.16123000207770621</v>
-      </c>
-      <c r="H30" s="48">
-        <f t="shared" si="22"/>
-        <v>9.0646806226516372E-2</v>
-      </c>
-      <c r="I30" s="48">
-        <f t="shared" si="22"/>
-        <v>0.11204757510509587</v>
-      </c>
-      <c r="J30" s="48">
-        <f t="shared" si="22"/>
-        <v>4.3482269634328496E-2</v>
-      </c>
-      <c r="K30" s="48">
-        <f t="shared" si="22"/>
-        <v>0.10193153904607065</v>
-      </c>
-      <c r="L30" s="48">
-        <f t="shared" si="22"/>
-        <v>6.6778927110897279E-2</v>
-      </c>
-      <c r="M30" s="48">
-        <f t="shared" si="22"/>
-        <v>5.2872111727476363E-2</v>
-      </c>
-      <c r="N30" s="48">
-        <f t="shared" si="22"/>
-        <v>7.0235307556113999E-2</v>
-      </c>
-      <c r="O30" s="48">
-        <f t="shared" si="22"/>
-        <v>0.25675405243145888</v>
-      </c>
-      <c r="P30" s="49">
-        <f t="shared" si="22"/>
-        <v>3.5031847133757961E-2</v>
-      </c>
-      <c r="Q30" s="50">
-        <f t="shared" si="22"/>
-        <v>2.910964102564105E-2</v>
-      </c>
-      <c r="R30" s="50">
-        <f t="shared" si="22"/>
-        <v>9.5911835762634304E-2</v>
-      </c>
-      <c r="S30" s="50">
-        <f t="shared" si="22"/>
-        <v>0.18568437532994464</v>
-      </c>
-      <c r="T30" s="50">
-        <f t="shared" si="22"/>
-        <v>5.0285319834330038E-2</v>
-      </c>
-      <c r="U30" s="50">
-        <f t="shared" si="22"/>
-        <v>4.6645430499751214E-2</v>
-      </c>
-      <c r="V30" s="50">
-        <f t="shared" si="22"/>
-        <v>9.4138765013851919E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22">
-      <c r="A31" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="30">
-        <f t="shared" ref="F31:P31" si="23">F7</f>
-        <v>138180</v>
-      </c>
-      <c r="G31" s="30">
-        <f t="shared" si="23"/>
-        <v>153056</v>
-      </c>
-      <c r="H31" s="30">
-        <f t="shared" si="23"/>
-        <v>169843</v>
-      </c>
-      <c r="I31" s="30">
-        <f t="shared" si="23"/>
-        <v>186210</v>
-      </c>
-      <c r="J31" s="30">
-        <f t="shared" si="23"/>
-        <v>204293</v>
-      </c>
-      <c r="K31" s="30">
-        <f t="shared" si="23"/>
-        <v>221936</v>
-      </c>
-      <c r="L31" s="30">
-        <f t="shared" si="23"/>
-        <v>239690</v>
-      </c>
-      <c r="M31" s="30">
-        <f t="shared" si="23"/>
-        <v>255497</v>
-      </c>
-      <c r="N31" s="30">
-        <f t="shared" si="23"/>
-        <v>273865</v>
-      </c>
-      <c r="O31" s="30">
-        <f t="shared" si="23"/>
-        <v>305710</v>
-      </c>
-      <c r="P31" s="51">
-        <f t="shared" si="23"/>
-        <v>336691</v>
-      </c>
-      <c r="Q31" s="33">
-        <f>P31*(1+Q32)</f>
-        <v>366993.19</v>
-      </c>
-      <c r="R31" s="52">
-        <v>402000</v>
-      </c>
-      <c r="S31" s="33">
-        <f>R31*(1+S32)</f>
-        <v>438180.00000000006</v>
-      </c>
-      <c r="T31" s="33">
-        <f>S31*(1+T32)</f>
-        <v>477616.20000000007</v>
-      </c>
-      <c r="U31" s="33">
-        <f>T31*(1+U32)</f>
-        <v>520601.65800000011</v>
-      </c>
-      <c r="V31" s="33">
-        <f>U31*(1+V32)</f>
-        <v>567455.80722000019</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22">
-      <c r="A32" s="53" t="s">
-        <v>168</v>
-      </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54">
-        <f t="shared" ref="G32:P32" si="24">(G31-F31)/F31</f>
-        <v>0.10765667969315386</v>
-      </c>
-      <c r="H32" s="54">
-        <f t="shared" si="24"/>
-        <v>0.10967881037006064</v>
-      </c>
-      <c r="I32" s="54">
-        <f t="shared" si="24"/>
-        <v>9.6365466931224719E-2</v>
-      </c>
-      <c r="J32" s="54">
-        <f t="shared" si="24"/>
-        <v>9.711078889425917E-2</v>
-      </c>
-      <c r="K32" s="54">
-        <f t="shared" si="24"/>
-        <v>8.6361255647525864E-2</v>
-      </c>
-      <c r="L32" s="54">
-        <f t="shared" si="24"/>
-        <v>7.9996034892942103E-2</v>
-      </c>
-      <c r="M32" s="54">
-        <f t="shared" si="24"/>
-        <v>6.5947682423129872E-2</v>
-      </c>
-      <c r="N32" s="54">
-        <f t="shared" si="24"/>
-        <v>7.1891255083229938E-2</v>
-      </c>
-      <c r="O32" s="54">
-        <f t="shared" si="24"/>
-        <v>0.11627991893816296</v>
-      </c>
-      <c r="P32" s="55">
-        <f t="shared" si="24"/>
-        <v>0.10134114029635929</v>
-      </c>
-      <c r="Q32" s="57">
-        <v>0.09</v>
-      </c>
-      <c r="R32" s="57">
-        <f>(R31-Q31)/Q31</f>
-        <v>9.5388173279182642E-2</v>
-      </c>
-      <c r="S32" s="58">
-        <v>0.09</v>
-      </c>
-      <c r="T32" s="58">
-        <v>0.09</v>
-      </c>
-      <c r="U32" s="58">
-        <v>0.09</v>
-      </c>
-      <c r="V32" s="58">
-        <v>0.09</v>
+      <c r="A28" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40">
+        <f>F8*80/96750</f>
+        <v>114.25736434108528</v>
+      </c>
+      <c r="G28" s="40">
+        <f>G8*80/96750</f>
+        <v>126.55793281653747</v>
+      </c>
+      <c r="H28" s="40">
+        <f>H8*80/96750</f>
+        <v>140.43865633074935</v>
+      </c>
+      <c r="I28" s="40">
+        <f>I8*80/96750</f>
+        <v>153.97209302325581</v>
+      </c>
+      <c r="J28" s="40">
+        <f>J8*80/96750</f>
+        <v>168.92444444444445</v>
+      </c>
+      <c r="K28" s="40">
+        <f>K8*80/96750</f>
+        <v>183.51297157622739</v>
+      </c>
+      <c r="L28" s="40">
+        <f>L8*80/96750</f>
+        <v>198.19328165374677</v>
+      </c>
+      <c r="M28" s="40">
+        <f>M8*80/96750</f>
+        <v>211.26366925064599</v>
+      </c>
+      <c r="N28" s="40">
+        <f>N8*80/96750</f>
+        <v>226.4516795865633</v>
+      </c>
+      <c r="O28" s="40">
+        <f>O8*80/96750</f>
+        <v>252.78346253229975</v>
+      </c>
+      <c r="P28" s="41">
+        <f>P8*80/96750</f>
+        <v>278.40082687338503</v>
+      </c>
+      <c r="Q28" s="40">
+        <f>Q8*80/96750</f>
+        <v>303.29311610565196</v>
+      </c>
+      <c r="R28" s="40">
+        <f>R8*80/96750</f>
+        <v>332.40310077519382</v>
+      </c>
+      <c r="S28" s="40">
+        <f>S8*80/96750</f>
+        <v>361.47887580606567</v>
+      </c>
+      <c r="T28" s="40">
+        <f>T8*80/96750</f>
+        <v>393.14811363427452</v>
+      </c>
+      <c r="U28" s="40">
+        <f>U8*80/96750</f>
+        <v>427.9660868269828</v>
+      </c>
+      <c r="V28" s="40">
+        <f>V8*80/96750</f>
+        <v>467.07737722966499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated for current quarter
</commit_message>
<xml_diff>
--- a/NCNO.xlsx
+++ b/NCNO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/specter/USEquities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AC33E7-64DE-9F47-8483-808AF2678FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47537FF4-F9E7-774E-B9EC-0443BD0C82D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Landing Page" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="170">
   <si>
     <t>Valuation Options: :</t>
   </si>
@@ -538,6 +538,9 @@
   </si>
   <si>
     <t>Actual:</t>
+  </si>
+  <si>
+    <t>H39 L28</t>
   </si>
   <si>
     <t>Narrative: NCNO has lumpy quarterly growth, but the growth in TTM revenue is steady. The estimations accomadate this by driving calculations off of TTM. 
@@ -548,7 +551,8 @@
 The Orange highlights represent Guidance Values
 The Teal range shown in the P/S ratio shows the price range for the trading period after the earnings announcement. (some discretion is used for edge values)
 When updating for quarterly reports, use 10Q data;
--Ensure quarterly trading range is accurate
+-Ensure quarterly high low is accurate
+-Ensure teal boxes are accurate
 -Move "Current" indicator
 -Update guidance values</t>
   </si>
@@ -598,7 +602,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -620,6 +624,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -666,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -712,11 +722,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -934,7 +945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBD4608-881B-F34A-AB93-66622F7714D7}">
   <dimension ref="A1:X1027"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:J36"/>
     </sheetView>
   </sheetViews>
@@ -946,18 +957,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="A1" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -968,16 +979,16 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -988,16 +999,16 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -1008,16 +1019,16 @@
       <c r="X3" s="1"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -1028,16 +1039,16 @@
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -1048,16 +1059,16 @@
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -1068,16 +1079,16 @@
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -1088,16 +1099,16 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="3"/>
       <c r="S8" s="1"/>
@@ -1108,16 +1119,16 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -1126,16 +1137,16 @@
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
@@ -1144,16 +1155,16 @@
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -1162,16 +1173,16 @@
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
       <c r="M12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1186,16 +1197,16 @@
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
       <c r="N13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1209,46 +1220,46 @@
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
       <c r="N14" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
       <c r="N15" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
       <c r="N16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1262,16 +1273,16 @@
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
       <c r="N17" s="3"/>
       <c r="Q17" s="8" t="s">
         <v>7</v>
@@ -1283,16 +1294,16 @@
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
       <c r="S18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="9" t="s">
@@ -1306,16 +1317,16 @@
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
       <c r="N19" s="1"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -1328,16 +1339,16 @@
       <c r="X19" s="3"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
       <c r="M20" s="5" t="s">
         <v>6</v>
       </c>
@@ -1355,16 +1366,16 @@
       <c r="X20" s="3"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
       <c r="M21" s="9" t="s">
         <v>8</v>
       </c>
@@ -1388,16 +1399,16 @@
       <c r="X21" s="3"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
       <c r="M22" s="9" t="s">
         <v>13</v>
       </c>
@@ -1418,16 +1429,16 @@
       <c r="X22" s="3"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
       <c r="M23" s="9" t="s">
         <v>17</v>
       </c>
@@ -1451,16 +1462,16 @@
       <c r="X23" s="3"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
       <c r="M24" s="9" t="s">
         <v>21</v>
       </c>
@@ -1482,16 +1493,16 @@
       <c r="X24" s="3"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
       <c r="M25" s="9" t="s">
         <v>25</v>
       </c>
@@ -1512,16 +1523,16 @@
       <c r="X25" s="3"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
       <c r="M26" s="9" t="s">
         <v>29</v>
       </c>
@@ -1544,16 +1555,16 @@
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
       <c r="M27" s="9" t="s">
         <v>32</v>
       </c>
@@ -1574,16 +1585,16 @@
       <c r="X27" s="3"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
       <c r="M28" s="9" t="s">
         <v>35</v>
       </c>
@@ -1604,16 +1615,16 @@
       <c r="X28" s="3"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
       <c r="M29" s="9" t="s">
         <v>38</v>
       </c>
@@ -1634,16 +1645,16 @@
       <c r="X29" s="3"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
       <c r="M30" s="9" t="s">
         <v>41</v>
       </c>
@@ -1662,16 +1673,16 @@
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
       <c r="M31" s="9" t="s">
         <v>44</v>
       </c>
@@ -1690,16 +1701,16 @@
       <c r="X31" s="1"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
       <c r="M32" s="9" t="s">
         <v>47</v>
       </c>
@@ -1718,16 +1729,16 @@
       <c r="X32" s="3"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
       <c r="M33" s="9" t="s">
         <v>50</v>
       </c>
@@ -1749,16 +1760,16 @@
       <c r="X33" s="3"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A34" s="27"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
       <c r="M34" s="9" t="s">
         <v>53</v>
       </c>
@@ -1777,16 +1788,16 @@
       <c r="X34" s="3"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
@@ -1799,16 +1810,16 @@
       <c r="X35" s="3"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A36" s="27"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
       <c r="M36" s="10" t="s">
         <v>57</v>
       </c>
@@ -13430,8 +13441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72C106E2-8288-6946-A55B-AB73FB561C12}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView topLeftCell="E1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13702,7 +13713,7 @@
       <c r="O5" s="13">
         <v>94200</v>
       </c>
-      <c r="P5" s="28">
+      <c r="P5" s="27">
         <v>99627</v>
       </c>
       <c r="Q5" s="23">
@@ -13777,7 +13788,7 @@
         <f t="shared" si="1"/>
         <v>305710</v>
       </c>
-      <c r="P6" s="29">
+      <c r="P6" s="28">
         <f t="shared" si="1"/>
         <v>338818</v>
       </c>
@@ -14105,7 +14116,7 @@
         <v>146</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
@@ -14246,7 +14257,7 @@
         <f t="shared" si="6"/>
         <v>23.698449612403103</v>
       </c>
-      <c r="P14" s="13">
+      <c r="P14" s="30">
         <f t="shared" si="6"/>
         <v>26.264961240310079</v>
       </c>

</xml_diff>